<commit_message>
Redo word2vec TransE evaluation due to missing values
</commit_message>
<xml_diff>
--- a/03_results_excel/evaluation_results.xlsx
+++ b/03_results_excel/evaluation_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vjola Cl\OneDrive - bwedu\MSC-WIWI\Masterarbeit\03_results_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E49B72-14F1-444F-BC44-967E48DC214A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D602E4-7826-4995-9B50-B3062AB3A320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransE_nations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Hits@10</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>transE</t>
+  </si>
+  <si>
+    <t>Word2Vec word embeddings</t>
   </si>
 </sst>
 </file>
@@ -344,25 +350,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -384,6 +380,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -667,7 +672,7 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,108 +687,119 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <v>0.94776099999999996</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="22">
         <v>4.7810949999999997</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="10">
         <v>0.28568199999999999</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="16">
         <v>0.94776099999999996</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <v>3.9154230000000001</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>0.46282699999999999</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="23"/>
+      <c r="B6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.94776099999999996</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4.7711439999999996</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.33170300000000003</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="16"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="18"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="16"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add BERT embeddings for wn18rr and fb15k237
</commit_message>
<xml_diff>
--- a/03_results_excel/evaluation_results.xlsx
+++ b/03_results_excel/evaluation_results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vjola Cl\OneDrive - bwedu\MSC-WIWI\Masterarbeit\03_results_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D602E4-7826-4995-9B50-B3062AB3A320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAE9010-136C-4383-BAC2-9CDAF3ABD392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransE_nations" sheetId="1" r:id="rId1"/>
+    <sheet name="WN18RR" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Hits@10</t>
   </si>
@@ -67,6 +68,42 @@
   </si>
   <si>
     <t>Word2Vec word embeddings</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimizer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">training approach </t>
+  </si>
+  <si>
+    <t>batch size</t>
+  </si>
+  <si>
+    <t>learning rate</t>
+  </si>
+  <si>
+    <t>nr epochs</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>initialization embeddings</t>
+  </si>
+  <si>
+    <t>BERT</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>sLCWA</t>
   </si>
 </sst>
 </file>
@@ -82,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,8 +132,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -344,13 +387,74 @@
         <color theme="0" tint="-0.499984740745262"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -380,6 +484,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,6 +495,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,16 +818,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
@@ -808,4 +939,175 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C36BE4-145E-46F6-BE1B-6442D962946B}">
+  <dimension ref="B2:G13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="0.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="0.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="E2" s="23"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="38">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E6" s="38">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="38">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="36">
+        <v>10</v>
+      </c>
+      <c r="E7" s="36">
+        <v>10</v>
+      </c>
+      <c r="G7" s="36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="35">
+        <v>128</v>
+      </c>
+      <c r="E8" s="35">
+        <v>128</v>
+      </c>
+      <c r="G8" s="35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="G11" s="19"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="G13" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>